<commit_message>
Deploying to gh-pages from @ ncpi-fhir/ncpi-fhir-ig-v0.2@4358b16 🚀
</commit_message>
<xml_diff>
--- a/CodeSystem-ConditionInheritanceMode.xlsx
+++ b/CodeSystem-ConditionInheritanceMode.xlsx
@@ -24,13 +24,13 @@
     <t>URL</t>
   </si>
   <si>
-    <t>https://ncpi-fhir.github.io/ncpi-fhir-ig/CodeSystem/ConditionInheritanceMode</t>
+    <t>https://ncpi-fhir.github.io/ncpi-fhir-ig-v02/CodeSystem/ConditionInheritanceMode</t>
   </si>
   <si>
     <t>Version</t>
   </si>
   <si>
-    <t>0.1.0</t>
+    <t>0.2.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2021-12-13T19:24:22+00:00</t>
+    <t>2022-05-26T12:34:56-05:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
Revert "Deploying to gh-pages from @ ncpi-fhir/ncpi-fhir-ig-v0.2@4358b16 🚀"
This reverts commit f2502adf2ac4be6c74e86c48bf327836cf41b2cf.
</commit_message>
<xml_diff>
--- a/CodeSystem-ConditionInheritanceMode.xlsx
+++ b/CodeSystem-ConditionInheritanceMode.xlsx
@@ -24,13 +24,13 @@
     <t>URL</t>
   </si>
   <si>
-    <t>https://ncpi-fhir.github.io/ncpi-fhir-ig-v02/CodeSystem/ConditionInheritanceMode</t>
+    <t>https://ncpi-fhir.github.io/ncpi-fhir-ig/CodeSystem/ConditionInheritanceMode</t>
   </si>
   <si>
     <t>Version</t>
   </si>
   <si>
-    <t>0.2.0</t>
+    <t>0.1.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-05-26T12:34:56-05:00</t>
+    <t>2021-12-13T19:24:22+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ ncpi-fhir/ncpi-fhir-ig-v0.2@ad3ee9b6e4b70dcbce6a9f3cc1a3aea4c35988c7 🚀
</commit_message>
<xml_diff>
--- a/CodeSystem-ConditionInheritanceMode.xlsx
+++ b/CodeSystem-ConditionInheritanceMode.xlsx
@@ -24,13 +24,13 @@
     <t>URL</t>
   </si>
   <si>
-    <t>https://ncpi-fhir.github.io/ncpi-fhir-ig/CodeSystem/ConditionInheritanceMode</t>
+    <t>https://ncpi-fhir.github.io/ncpi-fhir-ig-v02/CodeSystem/ConditionInheritanceMode</t>
   </si>
   <si>
     <t>Version</t>
   </si>
   <si>
-    <t>0.1.0</t>
+    <t>0.2.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2021-12-13T19:24:22+00:00</t>
+    <t>2022-05-26T18:07:50+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ ncpi-fhir/ncpi-fhir-ig-v0.2@13ca37311446ad84c18ac554bce2151064615887 🚀
</commit_message>
<xml_diff>
--- a/CodeSystem-ConditionInheritanceMode.xlsx
+++ b/CodeSystem-ConditionInheritanceMode.xlsx
@@ -24,7 +24,7 @@
     <t>URL</t>
   </si>
   <si>
-    <t>https://ncpi-fhir.github.io/ncpi-fhir-ig-v02/CodeSystem/ConditionInheritanceMode</t>
+    <t>https://nih-ncpi.github.io/ncpi-fhir-ig/CodeSystem/ConditionInheritanceMode</t>
   </si>
   <si>
     <t>Version</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-05-26T18:08:08+00:00</t>
+    <t>2022-05-26T18:29:57+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>